<commit_message>
changing and finalizing everything
</commit_message>
<xml_diff>
--- a/docs/text_data.xlsx
+++ b/docs/text_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianwalker/Dropbox (University of Oregon)/01_diabetes study/Diabetes Study/Real_Data_T1d_empowerment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianwalker/Documents/Everything/R_Tools22/diabetes_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB6797E-3021-A645-947B-BAA8345F4D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92944E8E-9AAF-0045-8340-8ADD7582834C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{130601AB-12E4-9E46-8065-14E85BC9B673}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Yes, definitely. I-- most of my experiences, it's like my legs start to get weak. When I was little, I used to say I'm wiggly, because that's really the only way that I could say “oh yeah, my blood sugar is going low.” Yeah, it's... I wouldn't say that it's like a too low. But it's it's like a, I would say it's like a lightheadedness. Kind of, not to the point that I need to sit down or I'm feeling super sick, but it's a feeling of something is not right. It's weird, like, those kinds of, with both my high blood sugar and with like dropping down really fast, it's not... I can't describe the feeling that it is other than it's my body just not... something doesn't feel right to me. Like I can name all of my-- I named all the feelings that I have when I go low. But I can't name any feelings of going high or anything. It's just like, it's just a feeling. A story that I like to say, because I just switched to Dexcom, probably two months ago, and there was a time that it was showing me like 110 or so or something like that just straight line. And then after like an hour or so I kind of thought to myself, you know, something doesn't feel right, I don't feel comfortable with this. Like, didn't feel high at all and I don't have like high symptoms. And I just decided to test myself and I was like 400, just... it was just a weird feeling of something doesn't feel right. And it's the same thing with like dropping down or going up really high really fast, where it's just like, something isn't right, I don't think this is good. And then I could check my Dexcom and it's like, oh, yeah, your two arrows going straight down, you got to do something. When I go start to start to go really low, my hands start to shake. I get super tired. And I just I can't really think straight and then I think the thing that's interesting is if I crash down and then immediately is stop myself from going low and Spike back up, I'm basically I'm sick for the rest the day. Like I just do not feel good. Something is off, and I just don't want to do anything. I mean, I feel like that it's a weird symptom, but it's like sometimes I feel like I just start losing the... the hearing. But like it goes, it doesn't go staticky, but it just feels like things are not in stereo or something. Everything feels weird and it just makes everything feel off. I mean, in some really rare cases where I've gone super low I just started like not understanding what things are, when things are happening. I've heard of people who had like rough times with their...with their low blood sugars and one person that I heard of swore that they were Batman to their roommates. But I've never had those like insane lows where I'm just not able to think properly, that I don't think I am who I am, or I just can't do anything like that. It's always been like, okay, something's off with my balance and my hearing...I can't really see straight even with glasses on. It's just kind of progresses and then it gets to the point that I'm like, I'm really tired. I can barely keep my eyes open. Something's wrong.</t>
   </si>
@@ -58,13 +58,59 @@
   </si>
   <si>
     <t>R_1fdCp8U6J7TIpPG</t>
+  </si>
+  <si>
+    <t>R_3nT0W62FHiaCGPg</t>
+  </si>
+  <si>
+    <t>So there's only been one time that I remember that it was happening, such that I was feeling confusion. And my family members that were with me at the time had to, you know, do things like say, Hey, quit holding your glucose and eat it, right? Like, but the most extreme ones, you know, pretty brutal, right? Like you. The best description I can give is, you kind of feel yourself fading, like, you know, you're gonna go unconscious in minutes if you don't do something. And then, you know, usually in an extreme low, like, where I get down into the 30s or lower, you know, sweating profusely shaky, no energy, you kind of get into that fight or flight mode, right? I've never actually used like glucagon, but I always keep glucagon on hand. Let me see really quick, let me look at Sugar made. And I could just, you know, sometimes it happens more. So let's see, over the last seven days, 12 lows, but that's a tough one, because that's anytime I went below seven, you know, from 60 to 70. Doesn't feel that bad for me. extreme lows. I don't I don't get them that often. That one time I was talking about with you. I think I hit a vein or hit muscle with my, my basal injection interest. So that's, you know, other times that I might have a low is usually low impact type exercise. So for example, in my conditioning days, I like to walk with a weight vest, that kind of activity. I rarely need insulin before the workout and I have to watch for a low mowing the lawn for whatever reason, I always have to make sure my, you know, I'm bringing my blood sugar up before I do that. Anyway, that's my thoughts and experiences on loads.So just about everything she's prescribing, she's also done. And I went in there prepared to ask her about doing it. And she was looking at this was shortly after I gone on to the dexcom, and she was looking at my numbers. And I was explaining Yun one of the reasons I wanted the decks calm was because of having lows in the middle of the night. I'm not sure why they're happening. And I'm worried about like never waking up from and. And that was when she said you should take your dose, split it in half, do two doses 12 hours apart. And then eventually you may want to tweak them. So for example, my morning dose is is larger than my evening dose. So and of course a lot of that has to do to with with how a person is eating, right. Depends on how much you might need. So So anyway, that's how I got to I had certain situations where I would do the basal insulin and then have these extreme loads. And then I had read online from people saying, Hey, watch out you're not getting muscle or hitting a vein or something because that'll definitely happen. When I started being really careful. Yeah, it seemed like that almost never happened.</t>
+  </si>
+  <si>
+    <t>R_1g6IuFecvJV6n6x</t>
+  </si>
+  <si>
+    <t>Sure. I mean, there are certainly times where I'm like, well, maybe I spoke to too much insulin, I didn't eat enough, I didn't do this. But there are I mean, I'd say 90% of the times. happened, there's been no explanation as to why these have occurred, except that I've had low blood sugar. I started having seizures when I was when I just graduated from college, and they were trying to correlate it with diabetes. But at that point, I didn't have a CGM, so there was no way to really determine that. And they still are not 100% sure that all of the teams are due to low blood sugar or that some of them are. But anytime that anyone has been an EMP has been called, my blood sugar has always been low enough, like in the 30s, where they've had to give me IV dextrose to bring it up. So I mean, the conclusion is that that's partly what's happening, but not 100%. Yeah, yeah. Like me and my coworker, my coworkers that I used to have, we were both type ones. And both of our husbands were like, You guys are the exact same when you get low like you get really mad which I'm sure you can understand, like, you know, when you go low, you just, you kind of just switch off and you're just like, I don't want that orange juice. I don't want because like, I'm fine, leave me alone. And they both would always say like, You guys are the exact same just like, we just want to leave you guys alone but we can't because you know if we leave you alone, it's gonna go lower and then you're just gonna like like great.</t>
+  </si>
+  <si>
+    <t>int_number</t>
+  </si>
+  <si>
+    <t>R_1mr573O3Ezhk8XJ</t>
+  </si>
+  <si>
+    <t>Yeah, so like the shakiness. sweatiness like lightheadedness. If it gets that bad, clearly my eyes my vision starts getting like spotty. Yeah, there's like sweaty, clammy, I guess like irritability. If someone's like asking me a stupid question, while I'm in the process of trying to drink the juice box, I could be irritable. Yeah, that's I would say though, like, I will also sometimes more often than not feel the actual act of how quick my blood sugar's dropping. So like, let's say, I have to correct for like being to 80 or something. I'm clearly not low. But if I am to AD, and I bolus correct, and it's like, double arrow down, or even one hour down, I'll get a sensation of low because of how quickly my blood sugar is dropping, if that makes sense. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oh I remember being I don't know what I was, I was like 10, nine or 10. I remember being in a hotel with my mom, my brother. I don't know what like led to the low. But I remember it was the first time I saw like, 20s on my glucometer I think it was like 21. And I remember being like, getting like, Yeah, I'm the shit. Like, I'm like, I'm still standing bro. Like, he can't touch me. I felt terrible. But I was also just like, you know, like, I'm Goku. And I'm Super Saiyan Three right now. But yeah, I felt terrible. Luckily, like, I came up, and like, everything was fine. But definitely, like, I think for my mom, she's like, let's not ever have that happen. I've been fortunate though, I haven't had a lot of like, terrible lows. Like, I don't know. I think as type ones, especially if you've very tight control on your relationship, like, you're constantly dipping into like very, very mild hybrid hypoglycemia, like, like 70s. I've, I've read studies before that, like in mice, you can condition their brains to be more resistant to the negative effects of severe hyperglycemia by exposing them repeatedly to mild hyperglycemia. Which doesn't mean it's good for your brain. But it is. It didn't make me like I was surprised because I've like read many stories about people being alone, just like they're just like, that's like when seizures and stuff started happening. And I was like, I was surprised that I was like, okay. Yeah, not the most exciting story but yeah. Oh, and how I feel? Yeah. I mean, like, one of the biggest things for me is I started to get visual Horace when I'm like, super low. Like, I always get like, really hungry, sweaty. I don't get like that. hunchy like, I've never been like super like mean or irritable when I'm low. But like, I dipped below, like 45. And I started to like, my, my whole visual field starts to change. And I'm like, like, Alexa play dangerous, don't like any logins. And like, I gotta get out there and get some of the that's how it feels to me. And like, sometimes I'll continue adding other symptoms, sometimes I'm just like, so hyper focused on getting to food and like, don't even pay attention symptoms. Yeah, like, if somebody if somebody just like subjected me to a study where they just continuously made me go low, and then it was like, the number one indicator for me being like, very, like, moderately to severely low versus just now there really is just like, I said, the visual stuff, and I started to like, sweat more. I get like, instead of like, okay, there's like a little bit of cumulating up here. It's like, I get cold, like cold sweat. Just like ready to rock. You know? I hate that feeling. Yeah, it's horrible. It's horrible. I had a once in a patient room and I was like, to my son working as a scribe. And it was same thing as like, oh, this visit is gonna last like five minutes and another five minutes max. I'm like, 60 right now. We'll make it or once we're done, I'll leave. I don't want to like leave in the middle of the note because then it's like, okay, well, I can't finish the note because I wasn't there for the whole visit. And they have to do it. And then Yeah, like 15 minutes later, I'm like, I'm sweating. I'm like, I gotta I don't know. I wish people understood type one better, because if they did, then it wouldn't be weird to just like, be like, Hey, I'm type one in my blood sugar. So I need to do this or like if I had a seizure disorder, and I was like, I feel like I'm about to have a seizure. I'm going to insert. This isn't a thing called like, like, nasal action, I think I think it might actually there is a nasal something for preventing seizures, but basically, like, if I think I pay like a 79 year old woman who's sitting there like talking to the doctor, if I was like, Yo, I'm about to have a seizure. I need to do this thing right now. Oh, yeah, do your thing. But I feel like diabetes is just like, because everyone latches on to. Everyone's like, Oh, I know, people with diabetes with type two. They don't who like it, they have lows. But like, it's just not as common like, certainly, like if you're insulin dependent, dependent type two diabetic, like, yeah, you're dealing with that. There's just not as commonly experienced by people with type two. I want to I don't want to belittle their struggles, because it's hard in a totally different way. But I just don't feel it talked about as much in the type twos that I've like, worked with, like I I feel like the loads they describe are like in like the 70s. Dude, I'll drive a car. No, I'm just kidding. </t>
+  </si>
+  <si>
+    <t>R_R3vFesQEw5vyUyB</t>
+  </si>
+  <si>
+    <t>I've only been like very low like three times, actually. And she's been nice. I'm super hyper aware for the most part. But yeah, the only ones where I've really gotten like very low, they actually kind of snuck up on me and it was kind of frightening. So like, the one time I just remember we were on family vacation. And I was young, like elementary school still. And everyone was during that whole thing where they argue over where to get lunch. And I was just getting like absurdly angry about it, which was fairly out of character for me to get like, super angry. To the point where I was like, just pick a restaurant. Like, oh my gosh, what's wrong with her? And so we got to the restaurant I checked, my blood sugar's like 30. And I was like, Oh, well, that explains a lot. My mom was also like, oh my gosh, and so luckily, I was able to go like, get a soft drink while we waited. But yeah. Like just that intense irritability. Mm hmm. Yeah. Yeah. </t>
+  </si>
+  <si>
+    <t>I've never passed out. I've gone down to 43. I think it's the lowest I've ever gone. And I feel horrible. When I go down to into the 40s, I've never passed out or come close to passing out I've always been alert. And I'm there very short, because I discovered something called SOS glucose powder. That if I take it within 15 minutes, I'm back. I'm up. So I don't stay in the lows very long, unless I'm distracting trying to get something else done. So, but I'm trying to think the worst low I've ever had. I ever the worst thing about being low is, let's say one time I was in New York City with my son. And my husband and I got super low. And so we just had to sit down until the stuff kicked in. And I didn't like that. And I don't want this to get in the way of our family, vacations and activities. So but I haven't had like a horrible situation where I was low and incapacitated, or Yeah, I have my alarm set. So when I hit 90, it goes up. So I'm able to monitor it and do something about it. And so you know, I may dip into the 60s, but I don't go super low. But sometimes I'll change it because you know, doing something right? Not my alarms going off at 90 and 80. And so I'll put it back down to 70. I may forget to put it back. And that's when I usually have my most because I've forgotten to put it </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um, let's see. I remember when I was and I don't remember my exact age, but I remember when when I was when I was, you know, a kid. And I remember it was the middle of the night and I somehow had had he was talking about seizures. I don't ever think I had never refer to any of this stuff as a seizure. I always think that but maybe it was I had fallen out of bed. And I guess I was like, kind of stuck under, between the, between the floor and the bed frame. And that's where my folks came in and found me. And I don't know, if we had glucagon back then. I think they probably tried to cram some glucose gel in my mouth. And then I ended took me took me took me down to the ER, is probably 20 minutes away. That's but that's really the only one I remember. I have been fortunate not to have a ton of them. Not to have a ton of real bad hypose I can usually feel it coming on. So unless you know, middle of the night is hard, but not these days with the next column. That was that was long before next time that was urine testing back then. Oh, it depends on what number we're looking at. But on the next, you know, if I've got a good calibrated sensor, I'll start feeling around 70. And then, it'll be a problem, you know, where I really have to, you know, and I could be like, have a walking low blood sugar at 70 and just go grab something to eat and just sort of go on about my business. But but but down around, like, you know, 160 55 that's when I have to sit down and wait it out. It's the 3am lows that get me in today. You probably don't know these when you maybe are struggling to correct some mistake made at dinnertime. And I always attend to rage bolus to try to fix that. And then it comes back at 3am It's 3am consistently that's the time of day get up and eat all the ice cream in the fridge that so that it affects my my sleep. And that happens. You know, maybe once every two weeks when I've done a stupid bitter thing and then over over compensated with the insulin and then it's like clockwork 3am and I eat the ice cream my wife 
+ </t>
+  </si>
+  <si>
+    <t>R_2TOeaDtBAd8rJgQ</t>
+  </si>
+  <si>
+    <t>R_1jTbJ73cP1sJNAX</t>
+  </si>
+  <si>
+    <t>R_2aEnOJSABPWYd6B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,14 +127,24 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,16 +167,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,51 +496,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67143C5-5493-CB49-94B8-FC25460AC058}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="301" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="371" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>